<commit_message>
Solving the problem with daylight saving time
</commit_message>
<xml_diff>
--- a/Video-EEG data.xlsx
+++ b/Video-EEG data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Kudlacek\FCD HFO\HFO long-term profile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kudlacek\Documents\GitHub\ALPACA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="602">
   <si>
     <t>Mouse</t>
   </si>
@@ -2993,6 +2993,21 @@
   </si>
   <si>
     <t>BogdaET725</t>
+  </si>
+  <si>
+    <t>CO006701</t>
+  </si>
+  <si>
+    <t>DQ</t>
+  </si>
+  <si>
+    <t>Carl Olson</t>
+  </si>
+  <si>
+    <t>CO006705</t>
+  </si>
+  <si>
+    <t>Birth date is made up</t>
   </si>
 </sst>
 </file>
@@ -3091,7 +3106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -3151,11 +3166,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3232,6 +3267,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -3450,10 +3489,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O172"/>
+  <dimension ref="A1:O174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="H174" sqref="H174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10127,6 +10166,43 @@
         <v>572</v>
       </c>
       <c r="O172" s="23"/>
+    </row>
+    <row r="173" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A173" s="44" t="s">
+        <v>597</v>
+      </c>
+      <c r="B173" s="48" t="s">
+        <v>598</v>
+      </c>
+      <c r="C173" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="D173" s="49" t="s">
+        <v>601</v>
+      </c>
+      <c r="G173" s="8">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A174" s="44" t="s">
+        <v>600</v>
+      </c>
+      <c r="B174" s="48" t="s">
+        <v>598</v>
+      </c>
+      <c r="C174" s="48" t="s">
+        <v>599</v>
+      </c>
+      <c r="D174" s="49" t="s">
+        <v>601</v>
+      </c>
+      <c r="E174" s="45"/>
+      <c r="F174" s="45"/>
+      <c r="G174" s="8">
+        <v>45901</v>
+      </c>
+      <c r="H174" s="45"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10474,31 +10550,31 @@
       <c r="O4" s="40"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="46" t="s">
         <v>589</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
       <c r="L5" s="40"/>
       <c r="M5" s="40"/>
       <c r="N5" s="40"/>
       <c r="O5" s="40"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="46" t="s">
         <v>590</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="40"/>
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>

</xml_diff>